<commit_message>
adding Protection Type to TM
</commit_message>
<xml_diff>
--- a/kerman/traffic_kerman.xlsx
+++ b/kerman/traffic_kerman.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\NetPlanner\kerman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\NetPlanner\NetPlanner\kerman\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="124">
   <si>
     <t>E1</t>
   </si>
@@ -557,6 +557,15 @@
   </si>
   <si>
     <t>Protection_Type</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Protection</t>
+  </si>
+  <si>
+    <t>Restoration</t>
   </si>
 </sst>
 </file>
@@ -1705,7 +1714,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1758,36 +1767,30 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="33" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="33" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="59" fillId="32" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="33" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="33" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="32" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="32" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="32" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="32" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="32" borderId="8" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1798,18 +1801,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2299,12 +2296,14 @@
   <dimension ref="A1:CG106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="1" max="8" width="8.88671875" style="31"/>
+    <col min="9" max="9" width="18.109375" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:85" ht="34.5" customHeight="1" thickBot="1">
@@ -2317,68 +2316,68 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30" t="s">
+      <c r="J1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30" t="s">
+      <c r="M1" s="27"/>
+      <c r="N1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="28" t="s">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="28" t="s">
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="28" t="s">
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="31" t="s">
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="32" t="s">
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="32" t="s">
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="32" t="s">
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="32" t="s">
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="33"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="30"/>
       <c r="AX1" s="15"/>
       <c r="AY1" s="15"/>
       <c r="AZ1" s="15"/>
@@ -2386,47 +2385,47 @@
       <c r="BB1" s="15"/>
       <c r="BC1" s="15"/>
       <c r="BD1" s="16"/>
-      <c r="BE1" s="26" t="s">
+      <c r="BE1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="BF1" s="27"/>
-      <c r="BG1" s="27"/>
-      <c r="BH1" s="31" t="s">
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="BI1" s="27"/>
-      <c r="BJ1" s="27"/>
-      <c r="BK1" s="31" t="s">
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="BL1" s="27"/>
-      <c r="BM1" s="27"/>
-      <c r="BN1" s="31" t="s">
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="BO1" s="27"/>
-      <c r="BP1" s="27"/>
-      <c r="BQ1" s="34" t="s">
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="BR1" s="34"/>
-      <c r="BS1" s="34"/>
-      <c r="BT1" s="34"/>
-      <c r="BU1" s="34"/>
-      <c r="BV1" s="34"/>
-      <c r="BW1" s="34"/>
-      <c r="BX1" s="34"/>
+      <c r="BR1" s="23"/>
+      <c r="BS1" s="23"/>
+      <c r="BT1" s="23"/>
+      <c r="BU1" s="23"/>
+      <c r="BV1" s="23"/>
+      <c r="BW1" s="23"/>
+      <c r="BX1" s="23"/>
       <c r="BY1" s="14"/>
-      <c r="BZ1" s="35" t="s">
+      <c r="BZ1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="CA1" s="35"/>
-      <c r="CB1" s="35"/>
-      <c r="CC1" s="35"/>
-      <c r="CD1" s="35"/>
-      <c r="CE1" s="35"/>
-      <c r="CF1" s="35"/>
-      <c r="CG1" s="35"/>
+      <c r="CA1" s="24"/>
+      <c r="CB1" s="24"/>
+      <c r="CC1" s="24"/>
+      <c r="CD1" s="24"/>
+      <c r="CE1" s="24"/>
+      <c r="CF1" s="24"/>
+      <c r="CG1" s="24"/>
     </row>
     <row r="2" spans="1:85" ht="80.400000000000006" thickBot="1">
       <c r="A2" s="7" t="s">
@@ -2684,2716 +2683,3023 @@
       </c>
     </row>
     <row r="3" spans="1:85">
-      <c r="A3" s="18">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="U3" s="21">
+      <c r="I3" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U3" s="20">
         <v>3</v>
       </c>
-      <c r="Y3" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="25">
+      <c r="Y3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:85">
-      <c r="A4" s="18">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="U4" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="24">
+      <c r="I4" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U4" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="20">
         <v>4</v>
       </c>
-      <c r="AL4" s="25">
+      <c r="AL4" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:85">
-      <c r="A5" s="18">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="U5" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="24">
+      <c r="I5" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U5" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="20">
         <v>8</v>
       </c>
-      <c r="AL5" s="25">
+      <c r="AL5" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:85">
-      <c r="A6" s="18">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="U6" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="22">
+      <c r="I6" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U6" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="20">
         <v>2</v>
       </c>
-      <c r="AC6" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="25">
+      <c r="AC6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:85">
-      <c r="A7" s="18">
+      <c r="A7" s="20">
         <v>5</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="U7" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="22">
+      <c r="I7" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U7" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="20">
         <v>3</v>
       </c>
-      <c r="AC7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="25">
+      <c r="AC7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:85">
-      <c r="A8" s="18">
+      <c r="A8" s="20">
         <v>6</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="U8" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="22">
+      <c r="I8" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U8" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="20">
         <v>2</v>
       </c>
-      <c r="AC8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="25">
+      <c r="AC8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:85">
-      <c r="A9" s="18">
+      <c r="A9" s="20">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="U9" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="24">
+      <c r="I9" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U9" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="20">
         <v>16</v>
       </c>
-      <c r="AL9" s="25">
+      <c r="AL9" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:85">
-      <c r="A10" s="18">
+      <c r="A10" s="20">
         <v>8</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="U10" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="24">
+      <c r="I10" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U10" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="20">
         <v>4</v>
       </c>
-      <c r="AL10" s="25">
+      <c r="AL10" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:85">
-      <c r="A11" s="18">
+      <c r="A11" s="20">
         <v>9</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="U11" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="24">
+      <c r="I11" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U11" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="20">
         <v>16</v>
       </c>
-      <c r="AL11" s="25">
+      <c r="AL11" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:85">
-      <c r="A12" s="18">
+      <c r="A12" s="20">
         <v>10</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="U12" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="22">
+      <c r="I12" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U12" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="20">
         <v>1</v>
       </c>
-      <c r="AC12" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="24">
+      <c r="AC12" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="20">
         <v>6</v>
       </c>
-      <c r="AL12" s="25">
+      <c r="AL12" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:85">
-      <c r="A13" s="18">
+      <c r="A13" s="20">
         <v>11</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="U13" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="24">
+      <c r="I13" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="U13" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="20">
         <v>20</v>
       </c>
-      <c r="AL13" s="25">
+      <c r="AL13" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:85">
-      <c r="A14" s="18">
+      <c r="A14" s="20">
         <v>12</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="U14" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="24">
+      <c r="I14" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U14" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="20">
         <v>37</v>
       </c>
-      <c r="AL14" s="25">
+      <c r="AL14" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:85">
-      <c r="A15" s="18">
+      <c r="A15" s="20">
         <v>13</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="U15" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="24">
+      <c r="I15" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U15" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="20">
         <v>8</v>
       </c>
-      <c r="AL15" s="25">
+      <c r="AL15" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:85">
-      <c r="A16" s="18">
+      <c r="A16" s="20">
         <v>14</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="U16" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="24">
+      <c r="I16" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U16" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="20">
         <v>6</v>
       </c>
-      <c r="AL16" s="25">
+      <c r="AL16" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:38">
-      <c r="A17" s="18">
+      <c r="A17" s="20">
         <v>15</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="U17" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="24">
+      <c r="I17" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U17" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="20">
         <v>18</v>
       </c>
-      <c r="AL17" s="25">
+      <c r="AL17" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:38">
-      <c r="A18" s="18">
+      <c r="A18" s="20">
         <v>16</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="U18" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="24">
+      <c r="I18" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U18" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="20">
         <v>63</v>
       </c>
-      <c r="AL18" s="25">
+      <c r="AL18" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:38">
-      <c r="A19" s="18">
+      <c r="A19" s="20">
         <v>17</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="U19" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="24">
+      <c r="I19" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U19" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="20">
         <v>4</v>
       </c>
-      <c r="AL19" s="25">
+      <c r="AL19" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:38">
-      <c r="A20" s="18">
+      <c r="A20" s="20">
         <v>18</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="U20" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="23">
+      <c r="I20" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U20" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="20">
         <v>8</v>
       </c>
-      <c r="AH20" s="24">
+      <c r="AH20" s="20">
         <v>4</v>
       </c>
-      <c r="AL20" s="25">
+      <c r="AL20" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:38">
-      <c r="A21" s="18">
+      <c r="A21" s="20">
         <v>19</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="U21" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH21" s="24">
+      <c r="I21" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U21" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="20">
         <v>4</v>
       </c>
-      <c r="AL21" s="25">
+      <c r="AL21" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:38">
-      <c r="A22" s="18">
+      <c r="A22" s="20">
         <v>20</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="U22" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH22" s="24">
+      <c r="I22" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U22" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="20">
         <v>4</v>
       </c>
-      <c r="AL22" s="25">
+      <c r="AL22" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:38">
-      <c r="A23" s="18">
+      <c r="A23" s="20">
         <v>21</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="U23" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="22">
+      <c r="I23" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U23" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="20">
         <v>3</v>
       </c>
-      <c r="AC23" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH23" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL23" s="25">
+      <c r="AC23" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:38">
-      <c r="A24" s="18">
+      <c r="A24" s="20">
         <v>22</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="U24" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="22">
+      <c r="I24" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U24" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="20">
         <v>1</v>
       </c>
-      <c r="AC24" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="24">
+      <c r="AC24" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="20">
         <v>2</v>
       </c>
-      <c r="AL24" s="25">
+      <c r="AL24" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:38">
-      <c r="A25" s="18">
+      <c r="A25" s="20">
         <v>23</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="U25" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="22">
+      <c r="I25" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U25" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="20">
         <v>1</v>
       </c>
-      <c r="AC25" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH25" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL25" s="25">
+      <c r="AC25" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:38">
-      <c r="A26" s="18">
+      <c r="A26" s="20">
         <v>24</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="U26" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="22">
+      <c r="I26" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U26" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="20">
         <v>1</v>
       </c>
-      <c r="AC26" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="24">
+      <c r="AC26" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="20">
         <v>6</v>
       </c>
-      <c r="AL26" s="25">
+      <c r="AL26" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:38">
-      <c r="A27" s="18">
+      <c r="A27" s="20">
         <v>25</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="U27" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH27" s="24">
+      <c r="I27" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U27" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="20">
         <v>9</v>
       </c>
-      <c r="AL27" s="25">
+      <c r="AL27" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:38">
-      <c r="A28" s="18">
+      <c r="A28" s="20">
         <v>26</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="U28" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH28" s="24">
+      <c r="I28" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U28" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="20">
         <v>4</v>
       </c>
-      <c r="AL28" s="25">
+      <c r="AL28" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:38">
-      <c r="A29" s="18">
+      <c r="A29" s="20">
         <v>27</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="U29" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="22">
+      <c r="I29" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="U29" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="20">
         <v>1</v>
       </c>
-      <c r="AC29" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH29" s="24">
+      <c r="AC29" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="20">
         <v>6</v>
       </c>
-      <c r="AL29" s="25">
+      <c r="AL29" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:38">
-      <c r="A30" s="18">
+      <c r="A30" s="20">
         <v>28</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="U30" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="22">
+      <c r="I30" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U30" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="20">
         <v>2</v>
       </c>
-      <c r="AC30" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH30" s="24">
+      <c r="AC30" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="20">
         <v>6</v>
       </c>
-      <c r="AL30" s="25">
+      <c r="AL30" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:38">
-      <c r="A31" s="18">
+      <c r="A31" s="20">
         <v>29</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="U31" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH31" s="24">
+      <c r="I31" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U31" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="20">
         <v>6</v>
       </c>
-      <c r="AL31" s="25">
+      <c r="AL31" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:38">
-      <c r="A32" s="18">
+      <c r="A32" s="20">
         <v>30</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="U32" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="22">
+      <c r="I32" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U32" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="20">
         <v>3</v>
       </c>
-      <c r="AC32" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH32" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL32" s="25">
+      <c r="AC32" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:38">
-      <c r="A33" s="18">
+      <c r="A33" s="20">
         <v>31</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="U33" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="22">
+      <c r="I33" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U33" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="20">
         <v>3</v>
       </c>
-      <c r="AC33" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH33" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL33" s="25">
+      <c r="AC33" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:38">
-      <c r="A34" s="18">
+      <c r="A34" s="20">
         <v>32</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="U34" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="22">
+      <c r="I34" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U34" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="20">
         <v>1</v>
       </c>
-      <c r="AC34" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH34" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL34" s="25">
+      <c r="AC34" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:38">
-      <c r="A35" s="18">
+      <c r="A35" s="20">
         <v>33</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="U35" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="22">
+      <c r="I35" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U35" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="20">
         <v>2</v>
       </c>
-      <c r="AC35" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH35" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL35" s="25">
+      <c r="AC35" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:38">
-      <c r="A36" s="18">
+      <c r="A36" s="20">
         <v>34</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="U36" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="22">
+      <c r="I36" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U36" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="20">
         <v>1</v>
       </c>
-      <c r="AC36" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH36" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL36" s="25">
+      <c r="AC36" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:38">
-      <c r="A37" s="18">
+      <c r="A37" s="20">
         <v>35</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="U37" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="22">
+      <c r="I37" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U37" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="20">
         <v>1</v>
       </c>
-      <c r="AC37" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH37" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL37" s="25">
+      <c r="AC37" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:38">
-      <c r="A38" s="18">
+      <c r="A38" s="20">
         <v>36</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="U38" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="22">
+      <c r="I38" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U38" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="20">
         <v>2</v>
       </c>
-      <c r="AC38" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH38" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL38" s="25">
+      <c r="AC38" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:38">
-      <c r="A39" s="18">
+      <c r="A39" s="20">
         <v>37</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="U39" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="22">
+      <c r="I39" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U39" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="20">
         <v>1</v>
       </c>
-      <c r="AC39" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH39" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL39" s="25">
+      <c r="AC39" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:38">
-      <c r="A40" s="18">
+      <c r="A40" s="20">
         <v>38</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="U40" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH40" s="24">
+      <c r="I40" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U40" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="20">
         <v>8</v>
       </c>
-      <c r="AL40" s="25">
+      <c r="AL40" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:38">
-      <c r="A41" s="18">
+      <c r="A41" s="20">
         <v>39</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="U41" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="23">
+      <c r="I41" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U41" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="20">
         <v>2</v>
       </c>
-      <c r="AH41" s="24">
+      <c r="AH41" s="20">
         <v>16</v>
       </c>
-      <c r="AL41" s="25">
+      <c r="AL41" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:38">
-      <c r="A42" s="18">
+      <c r="A42" s="20">
         <v>40</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="U42" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH42" s="24">
+      <c r="I42" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U42" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="20">
         <v>4</v>
       </c>
-      <c r="AL42" s="25">
+      <c r="AL42" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:38">
-      <c r="A43" s="18">
+      <c r="A43" s="20">
         <v>41</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="U43" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH43" s="24">
+      <c r="I43" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U43" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="20">
         <v>4</v>
       </c>
-      <c r="AL43" s="25">
+      <c r="AL43" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:38">
-      <c r="A44" s="18">
+      <c r="A44" s="20">
         <v>42</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="U44" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH44" s="24">
+      <c r="I44" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U44" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH44" s="20">
         <v>4</v>
       </c>
-      <c r="AL44" s="25">
+      <c r="AL44" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:38">
-      <c r="A45" s="18">
+      <c r="A45" s="20">
         <v>43</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="U45" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH45" s="24">
+      <c r="I45" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U45" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH45" s="20">
         <v>4</v>
       </c>
-      <c r="AL45" s="25">
+      <c r="AL45" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:38">
-      <c r="A46" s="18">
+      <c r="A46" s="20">
         <v>44</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="U46" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC46" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH46" s="24">
+      <c r="I46" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U46" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="20">
         <v>4</v>
       </c>
-      <c r="AL46" s="25">
+      <c r="AL46" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:38">
-      <c r="A47" s="18">
+      <c r="A47" s="20">
         <v>45</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="U47" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC47" s="23">
+      <c r="I47" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U47" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="20">
         <v>2</v>
       </c>
-      <c r="AH47" s="24">
+      <c r="AH47" s="20">
         <v>6</v>
       </c>
-      <c r="AL47" s="25">
+      <c r="AL47" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:38">
-      <c r="A48" s="18">
+      <c r="A48" s="20">
         <v>46</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="U48" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y48" s="22">
+      <c r="I48" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U48" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="20">
         <v>2</v>
       </c>
-      <c r="AC48" s="23">
+      <c r="AC48" s="20">
         <v>1</v>
       </c>
-      <c r="AH48" s="24">
+      <c r="AH48" s="20">
         <v>4</v>
       </c>
-      <c r="AL48" s="25">
+      <c r="AL48" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:38">
-      <c r="A49" s="18">
+      <c r="A49" s="20">
         <v>47</v>
       </c>
-      <c r="B49" s="19" t="s">
+      <c r="B49" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="U49" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y49" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC49" s="23">
+      <c r="I49" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U49" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="20">
         <v>3</v>
       </c>
-      <c r="AH49" s="24">
+      <c r="AH49" s="20">
         <v>10</v>
       </c>
-      <c r="AL49" s="25">
+      <c r="AL49" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:38">
-      <c r="A50" s="18">
+      <c r="A50" s="20">
         <v>48</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="U50" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC50" s="23">
+      <c r="I50" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U50" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="20">
         <v>4</v>
       </c>
-      <c r="AH50" s="24">
+      <c r="AH50" s="20">
         <v>8</v>
       </c>
-      <c r="AL50" s="25">
+      <c r="AL50" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:38">
-      <c r="A51" s="18">
+      <c r="A51" s="20">
         <v>49</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="U51" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC51" s="23">
+      <c r="I51" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U51" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="20">
         <v>1</v>
       </c>
-      <c r="AH51" s="24">
+      <c r="AH51" s="20">
         <v>2</v>
       </c>
-      <c r="AL51" s="25">
+      <c r="AL51" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:38">
-      <c r="A52" s="18">
+      <c r="A52" s="20">
         <v>50</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="U52" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y52" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC52" s="23">
+      <c r="I52" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U52" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="20">
         <v>1</v>
       </c>
-      <c r="AH52" s="24">
+      <c r="AH52" s="20">
         <v>4</v>
       </c>
-      <c r="AL52" s="25">
+      <c r="AL52" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:38">
-      <c r="A53" s="18">
+      <c r="A53" s="20">
         <v>51</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="U53" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y53" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC53" s="23">
+      <c r="I53" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U53" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="20">
         <v>2</v>
       </c>
-      <c r="AH53" s="24">
+      <c r="AH53" s="20">
         <v>6</v>
       </c>
-      <c r="AL53" s="25">
+      <c r="AL53" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:38">
-      <c r="A54" s="18">
+      <c r="A54" s="20">
         <v>52</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="U54" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y54" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC54" s="23">
+      <c r="I54" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U54" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="20">
         <v>1</v>
       </c>
-      <c r="AH54" s="24">
+      <c r="AH54" s="20">
         <v>4</v>
       </c>
-      <c r="AL54" s="25">
+      <c r="AL54" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:38">
-      <c r="A55" s="18">
+      <c r="A55" s="20">
         <v>53</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="U55" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y55" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC55" s="23">
+      <c r="I55" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U55" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y55" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="20">
         <v>4</v>
       </c>
-      <c r="AH55" s="24">
+      <c r="AH55" s="20">
         <v>14</v>
       </c>
-      <c r="AL55" s="25">
+      <c r="AL55" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:38">
-      <c r="A56" s="18">
+      <c r="A56" s="20">
         <v>54</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B56" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="U56" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y56" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC56" s="23">
+      <c r="I56" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U56" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="20">
         <v>3</v>
       </c>
-      <c r="AH56" s="24">
+      <c r="AH56" s="20">
         <v>2</v>
       </c>
-      <c r="AL56" s="25">
+      <c r="AL56" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:38">
-      <c r="A57" s="18">
+      <c r="A57" s="20">
         <v>55</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="U57" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC57" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH57" s="24">
+      <c r="I57" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U57" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC57" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH57" s="20">
         <v>4</v>
       </c>
-      <c r="AL57" s="25">
+      <c r="AL57" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:38">
-      <c r="A58" s="18">
+      <c r="A58" s="20">
         <v>56</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="U58" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y58" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC58" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH58" s="24">
+      <c r="I58" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U58" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y58" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC58" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH58" s="20">
         <v>4</v>
       </c>
-      <c r="AL58" s="25">
+      <c r="AL58" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:38">
-      <c r="A59" s="18">
+      <c r="A59" s="20">
         <v>57</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="U59" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC59" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH59" s="24">
+      <c r="I59" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U59" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC59" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH59" s="20">
         <v>4</v>
       </c>
-      <c r="AL59" s="25">
+      <c r="AL59" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:38">
-      <c r="A60" s="18">
+      <c r="A60" s="20">
         <v>58</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="U60" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC60" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH60" s="24">
+      <c r="I60" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U60" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH60" s="20">
         <v>4</v>
       </c>
-      <c r="AL60" s="25">
+      <c r="AL60" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:38">
-      <c r="A61" s="18">
+      <c r="A61" s="20">
         <v>59</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="U61" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC61" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH61" s="24">
+      <c r="I61" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U61" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH61" s="20">
         <v>4</v>
       </c>
-      <c r="AL61" s="25">
+      <c r="AL61" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:38">
-      <c r="A62" s="18">
+      <c r="A62" s="20">
         <v>60</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="U62" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH62" s="24">
+      <c r="I62" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U62" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="20">
         <v>4</v>
       </c>
-      <c r="AL62" s="25">
+      <c r="AL62" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:38">
-      <c r="A63" s="18">
+      <c r="A63" s="20">
         <v>61</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="U63" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y63" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC63" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH63" s="24">
+      <c r="I63" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U63" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC63" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH63" s="20">
         <v>4</v>
       </c>
-      <c r="AL63" s="25">
+      <c r="AL63" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:38">
-      <c r="A64" s="18">
+      <c r="A64" s="20">
         <v>62</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="U64" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y64" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC64" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH64" s="24">
+      <c r="I64" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U64" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="20">
         <v>4</v>
       </c>
-      <c r="AL64" s="25">
+      <c r="AL64" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:38">
-      <c r="A65" s="18">
+      <c r="A65" s="20">
         <v>63</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="U65" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y65" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC65" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH65" s="24">
+      <c r="I65" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U65" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH65" s="20">
         <v>4</v>
       </c>
-      <c r="AL65" s="25">
+      <c r="AL65" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:38">
-      <c r="A66" s="18">
+      <c r="A66" s="20">
         <v>64</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="U66" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y66" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC66" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH66" s="24">
+      <c r="I66" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U66" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH66" s="20">
         <v>4</v>
       </c>
-      <c r="AL66" s="25">
+      <c r="AL66" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:38">
-      <c r="A67" s="18">
+      <c r="A67" s="20">
         <v>65</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="B67" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="U67" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y67" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC67" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH67" s="24">
+      <c r="I67" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U67" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="20">
         <v>19</v>
       </c>
-      <c r="AL67" s="25">
+      <c r="AL67" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:38">
-      <c r="A68" s="18">
+      <c r="A68" s="20">
         <v>66</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="U68" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y68" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC68" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH68" s="24">
+      <c r="I68" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U68" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC68" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH68" s="20">
         <v>2</v>
       </c>
-      <c r="AL68" s="25">
+      <c r="AL68" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:38">
-      <c r="A69" s="18">
+      <c r="A69" s="20">
         <v>67</v>
       </c>
-      <c r="B69" s="19" t="s">
+      <c r="B69" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="U69" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y69" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC69" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH69" s="24">
+      <c r="I69" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U69" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC69" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH69" s="20">
         <v>61</v>
       </c>
-      <c r="AL69" s="25">
+      <c r="AL69" s="20">
         <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:38">
-      <c r="A70" s="18">
+      <c r="A70" s="20">
         <v>68</v>
       </c>
-      <c r="B70" s="19" t="s">
+      <c r="B70" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="U70" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y70" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC70" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH70" s="24">
+      <c r="I70" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U70" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y70" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC70" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH70" s="20">
         <v>7</v>
       </c>
-      <c r="AL70" s="25">
+      <c r="AL70" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:38">
-      <c r="A71" s="18">
+      <c r="A71" s="20">
         <v>69</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="U71" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y71" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC71" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH71" s="24">
+      <c r="I71" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U71" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y71" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC71" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH71" s="20">
         <v>12</v>
       </c>
-      <c r="AL71" s="25">
+      <c r="AL71" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:38">
-      <c r="A72" s="18">
+      <c r="A72" s="20">
         <v>70</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C72" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="U72" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y72" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC72" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH72" s="24">
+      <c r="I72" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U72" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y72" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="20">
         <v>4</v>
       </c>
-      <c r="AL72" s="25">
+      <c r="AL72" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:38">
-      <c r="A73" s="18">
+      <c r="A73" s="20">
         <v>71</v>
       </c>
-      <c r="B73" s="19" t="s">
+      <c r="B73" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C73" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="U73" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y73" s="22">
+      <c r="I73" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U73" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y73" s="20">
         <v>3</v>
       </c>
-      <c r="AC73" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH73" s="24">
+      <c r="AC73" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH73" s="20">
         <v>18</v>
       </c>
-      <c r="AL73" s="25">
+      <c r="AL73" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:38">
-      <c r="A74" s="18">
+      <c r="A74" s="20">
         <v>72</v>
       </c>
-      <c r="B74" s="19" t="s">
+      <c r="B74" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="U74" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y74" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC74" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH74" s="24">
+      <c r="I74" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U74" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y74" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC74" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH74" s="20">
         <v>18</v>
       </c>
-      <c r="AL74" s="25">
+      <c r="AL74" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:38">
-      <c r="A75" s="18">
+      <c r="A75" s="20">
         <v>73</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B75" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="U75" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y75" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC75" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH75" s="24">
+      <c r="I75" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U75" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y75" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC75" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH75" s="20">
         <v>4</v>
       </c>
-      <c r="AL75" s="25">
+      <c r="AL75" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:38">
-      <c r="A76" s="18">
+      <c r="A76" s="20">
         <v>74</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="B76" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C76" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="U76" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y76" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC76" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH76" s="24">
+      <c r="I76" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U76" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y76" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC76" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH76" s="20">
         <v>4</v>
       </c>
-      <c r="AL76" s="25">
+      <c r="AL76" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:38">
-      <c r="A77" s="18">
+      <c r="A77" s="20">
         <v>75</v>
       </c>
-      <c r="B77" s="19" t="s">
+      <c r="B77" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C77" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="U77" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y77" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC77" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH77" s="24">
+      <c r="I77" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U77" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y77" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC77" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH77" s="20">
         <v>4</v>
       </c>
-      <c r="AL77" s="25">
+      <c r="AL77" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:38">
-      <c r="A78" s="18">
+      <c r="A78" s="20">
         <v>76</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B78" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="U78" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y78" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC78" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH78" s="24">
+      <c r="I78" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U78" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH78" s="20">
         <v>4</v>
       </c>
-      <c r="AL78" s="25">
+      <c r="AL78" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:38">
-      <c r="A79" s="18">
+      <c r="A79" s="20">
         <v>77</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="B79" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="U79" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y79" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC79" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH79" s="24">
+      <c r="I79" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U79" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y79" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC79" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH79" s="20">
         <v>4</v>
       </c>
-      <c r="AL79" s="25">
+      <c r="AL79" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:38">
-      <c r="A80" s="18">
+      <c r="A80" s="20">
         <v>78</v>
       </c>
-      <c r="B80" s="19" t="s">
+      <c r="B80" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="U80" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y80" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC80" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH80" s="24">
+      <c r="I80" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U80" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y80" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC80" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH80" s="20">
         <v>4</v>
       </c>
-      <c r="AL80" s="25">
+      <c r="AL80" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:38">
-      <c r="A81" s="18">
+      <c r="A81" s="20">
         <v>79</v>
       </c>
-      <c r="B81" s="19" t="s">
+      <c r="B81" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="U81" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC81" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH81" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL81" s="25">
+      <c r="I81" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U81" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y81" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC81" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH81" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL81" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:38">
-      <c r="A82" s="18">
+      <c r="A82" s="20">
         <v>80</v>
       </c>
-      <c r="B82" s="19" t="s">
+      <c r="B82" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="U82" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y82" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC82" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH82" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL82" s="25">
+      <c r="I82" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U82" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC82" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:38">
-      <c r="A83" s="18">
+      <c r="A83" s="20">
         <v>81</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="B83" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="C83" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="U83" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y83" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC83" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH83" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL83" s="25">
+      <c r="I83" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U83" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y83" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC83" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:38">
-      <c r="A84" s="18">
+      <c r="A84" s="20">
         <v>82</v>
       </c>
-      <c r="B84" s="19" t="s">
+      <c r="B84" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="U84" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y84" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC84" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH84" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL84" s="25">
+      <c r="I84" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U84" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y84" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC84" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH84" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL84" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:38">
-      <c r="A85" s="18">
+      <c r="A85" s="20">
         <v>83</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="B85" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="U85" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y85" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC85" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH85" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL85" s="25">
+      <c r="I85" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U85" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y85" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC85" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH85" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL85" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:38">
-      <c r="A86" s="18">
+      <c r="A86" s="20">
         <v>84</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="U86" s="21">
+      <c r="I86" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U86" s="20">
         <v>1</v>
       </c>
-      <c r="Y86" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC86" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH86" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL86" s="25">
+      <c r="Y86" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC86" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH86" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL86" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:38">
-      <c r="A87" s="18">
+      <c r="A87" s="20">
         <v>85</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B87" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C87" s="19" t="s">
+      <c r="C87" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="U87" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y87" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC87" s="23">
+      <c r="I87" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U87" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y87" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC87" s="20">
         <v>4</v>
       </c>
-      <c r="AH87" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL87" s="25">
+      <c r="AH87" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL87" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:38">
-      <c r="A88" s="18">
+      <c r="A88" s="20">
         <v>86</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="U88" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y88" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC88" s="23">
+      <c r="I88" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U88" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y88" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC88" s="20">
         <v>4</v>
       </c>
-      <c r="AH88" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL88" s="25">
+      <c r="AH88" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL88" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:38">
-      <c r="A89" s="18">
+      <c r="A89" s="20">
         <v>87</v>
       </c>
-      <c r="B89" s="20" t="s">
+      <c r="B89" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C89" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="U89" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y89" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC89" s="23">
+      <c r="I89" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U89" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y89" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC89" s="20">
         <v>4</v>
       </c>
-      <c r="AH89" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL89" s="25">
+      <c r="AH89" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL89" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:38">
-      <c r="A90" s="18">
+      <c r="A90" s="20">
         <v>88</v>
       </c>
-      <c r="B90" s="19" t="s">
+      <c r="B90" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="U90" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y90" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC90" s="23">
+      <c r="I90" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U90" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y90" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC90" s="20">
         <v>4</v>
       </c>
-      <c r="AH90" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL90" s="25">
+      <c r="AH90" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL90" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:38">
-      <c r="A91" s="18">
+      <c r="A91" s="20">
         <v>89</v>
       </c>
-      <c r="B91" s="19" t="s">
+      <c r="B91" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="U91" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y91" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC91" s="23">
+      <c r="I91" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U91" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y91" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC91" s="20">
         <v>12</v>
       </c>
-      <c r="AH91" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL91" s="25">
+      <c r="AH91" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL91" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:38">
-      <c r="A92" s="18">
+      <c r="A92" s="20">
         <v>90</v>
       </c>
-      <c r="B92" s="19" t="s">
+      <c r="B92" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C92" s="19" t="s">
+      <c r="C92" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="U92" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y92" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC92" s="23">
+      <c r="I92" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U92" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC92" s="20">
         <v>4</v>
       </c>
-      <c r="AH92" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL92" s="25">
+      <c r="AH92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL92" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:38">
-      <c r="A93" s="18">
+      <c r="A93" s="20">
         <v>91</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B93" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="U93" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y93" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC93" s="23">
+      <c r="I93" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U93" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y93" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC93" s="20">
         <v>20</v>
       </c>
-      <c r="AH93" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL93" s="25">
+      <c r="AH93" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL93" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:38">
-      <c r="A94" s="18">
+      <c r="A94" s="20">
         <v>92</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="B94" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="C94" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="U94" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y94" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC94" s="23">
+      <c r="I94" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U94" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC94" s="20">
         <v>4</v>
       </c>
-      <c r="AH94" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL94" s="25">
+      <c r="AH94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL94" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:38">
-      <c r="A95" s="18">
+      <c r="A95" s="20">
         <v>93</v>
       </c>
-      <c r="B95" s="19" t="s">
+      <c r="B95" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="U95" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y95" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC95" s="23">
+      <c r="I95" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U95" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y95" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC95" s="20">
         <v>4</v>
       </c>
-      <c r="AH95" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL95" s="25">
+      <c r="AH95" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL95" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:38">
-      <c r="A96" s="18">
+      <c r="A96" s="20">
         <v>94</v>
       </c>
-      <c r="B96" s="19" t="s">
+      <c r="B96" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="U96" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y96" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC96" s="23">
+      <c r="I96" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U96" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y96" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC96" s="20">
         <v>4</v>
       </c>
-      <c r="AH96" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL96" s="25">
+      <c r="AH96" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL96" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:38">
-      <c r="A97" s="18">
+      <c r="A97" s="20">
         <v>95</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B97" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C97" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="U97" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y97" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC97" s="23">
+      <c r="I97" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U97" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y97" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC97" s="20">
         <v>8</v>
       </c>
-      <c r="AH97" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL97" s="25">
+      <c r="AH97" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL97" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:38">
-      <c r="A98" s="18">
+      <c r="A98" s="20">
         <v>96</v>
       </c>
-      <c r="B98" s="20" t="s">
+      <c r="B98" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C98" s="20" t="s">
+      <c r="C98" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="U98" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y98" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC98" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH98" s="24">
+      <c r="I98" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U98" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y98" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC98" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH98" s="20">
         <v>6</v>
       </c>
-      <c r="AL98" s="25">
+      <c r="AL98" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:38">
-      <c r="A99" s="18">
+      <c r="A99" s="20">
         <v>97</v>
       </c>
-      <c r="B99" s="20" t="s">
+      <c r="B99" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C99" s="20" t="s">
+      <c r="C99" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="U99" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y99" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC99" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH99" s="24">
+      <c r="I99" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U99" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y99" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC99" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH99" s="20">
         <v>8</v>
       </c>
-      <c r="AL99" s="25">
+      <c r="AL99" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:38">
-      <c r="A100" s="18">
+      <c r="A100" s="20">
         <v>98</v>
       </c>
-      <c r="B100" s="20" t="s">
+      <c r="B100" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C100" s="20" t="s">
+      <c r="C100" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="U100" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y100" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC100" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH100" s="24">
+      <c r="I100" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U100" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y100" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC100" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH100" s="20">
         <v>6</v>
       </c>
-      <c r="AL100" s="25">
+      <c r="AL100" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:38">
-      <c r="A101" s="18">
+      <c r="A101" s="20">
         <v>99</v>
       </c>
-      <c r="B101" s="20" t="s">
+      <c r="B101" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="C101" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="U101" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y101" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC101" s="23">
+      <c r="I101" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U101" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y101" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC101" s="20">
         <v>4</v>
       </c>
-      <c r="AH101" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL101" s="25">
+      <c r="AH101" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL101" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:38">
-      <c r="A102" s="18">
+      <c r="A102" s="20">
         <v>100</v>
       </c>
-      <c r="B102" s="20" t="s">
+      <c r="B102" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C102" s="20" t="s">
+      <c r="C102" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="U102" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y102" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC102" s="23">
+      <c r="I102" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U102" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y102" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC102" s="20">
         <v>4</v>
       </c>
-      <c r="AH102" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL102" s="25">
+      <c r="AH102" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL102" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:38">
-      <c r="A103" s="18">
+      <c r="A103" s="20">
         <v>101</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B103" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C103" s="20" t="s">
+      <c r="C103" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="U103" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y103" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC103" s="23">
+      <c r="I103" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U103" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y103" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC103" s="20">
         <v>1</v>
       </c>
-      <c r="AH103" s="24">
-        <v>0</v>
-      </c>
-      <c r="AL103" s="25">
+      <c r="AH103" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL103" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:38">
-      <c r="A104" s="18">
+      <c r="A104" s="20">
         <v>102</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="B104" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="C104" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="U104" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y104" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC104" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH104" s="24">
+      <c r="I104" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U104" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y104" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC104" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH104" s="20">
         <v>4</v>
       </c>
-      <c r="AL104" s="25">
+      <c r="AL104" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:38">
-      <c r="A105" s="18">
+      <c r="A105" s="20">
         <v>103</v>
       </c>
-      <c r="B105" s="20" t="s">
+      <c r="B105" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C105" s="20" t="s">
+      <c r="C105" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="U105" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y105" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC105" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH105" s="24">
+      <c r="I105" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U105" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y105" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC105" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH105" s="20">
         <v>4</v>
       </c>
-      <c r="AL105" s="25">
+      <c r="AL105" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:38">
-      <c r="A106" s="18">
+      <c r="A106" s="20">
         <v>104</v>
       </c>
-      <c r="B106" s="20" t="s">
+      <c r="B106" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="U106" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y106" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC106" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH106" s="24">
+      <c r="I106" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="U106" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y106" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC106" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH106" s="20">
         <v>4</v>
       </c>
-      <c r="AL106" s="25">
+      <c r="AL106" s="20">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BH1:BJ1"/>
-    <mergeCell ref="BK1:BM1"/>
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BQ1:BX1"/>
-    <mergeCell ref="BZ1:CG1"/>
     <mergeCell ref="BE1:BG1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
@@ -5406,6 +5712,11 @@
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="BH1:BJ1"/>
+    <mergeCell ref="BK1:BM1"/>
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BQ1:BX1"/>
+    <mergeCell ref="BZ1:CG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>